<commit_message>
Planilha finalizada; Adicionada melhor resolução de tempo.
</commit_message>
<xml_diff>
--- a/Pratica/Projects/lab1/Lab1_2019_2.xlsx
+++ b/Pratica/Projects/lab1/Lab1_2019_2.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAELN\Downloads\Embarcados-master\Pratica\Projects\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davi\Desktop\GIT\Embarcados\Pratica\Projects\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFB8188-216C-45C7-904C-9C231C85A3FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Ciclo de trabalho (%)</t>
   </si>
@@ -84,12 +92,15 @@
   </si>
   <si>
     <t>f_sinal = 1kHz</t>
+  </si>
+  <si>
+    <t>203 ns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -190,7 +201,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -228,7 +239,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -263,6 +274,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -298,9 +326,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,11 +518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,6 +1684,9 @@
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1655,7 +1703,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1667,7 +1715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>